<commit_message>
Murdoch's label, need to think through eaches (24, 40, 6) and their relationship to quantities and skus
</commit_message>
<xml_diff>
--- a/Finished/Murdochs/671521438/Murdochs 856 ASN PO 671521438 10.22.2024.xlsx
+++ b/Finished/Murdochs/671521438/Murdochs 856 ASN PO 671521438 10.22.2024.xlsx
@@ -1255,7 +1255,11 @@
           <t>10/18/2024</t>
         </is>
       </c>
-      <c r="D20" s="33" t="n"/>
+      <c r="D20" s="33" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
       <c r="E20" s="33" t="n"/>
       <c r="F20" s="34" t="inlineStr">
         <is>
@@ -1304,7 +1308,11 @@
           <t>10/18/2024</t>
         </is>
       </c>
-      <c r="D21" s="33" t="n"/>
+      <c r="D21" s="33" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
       <c r="E21" s="33" t="n"/>
       <c r="F21" s="34" t="inlineStr">
         <is>
@@ -1353,7 +1361,11 @@
           <t>10/18/2024</t>
         </is>
       </c>
-      <c r="D22" s="33" t="n"/>
+      <c r="D22" s="33" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
       <c r="E22" s="33" t="n"/>
       <c r="F22" s="34" t="inlineStr">
         <is>

</xml_diff>